<commit_message>
Mejora en crearOrden, pasado a Object Model
</commit_message>
<xml_diff>
--- a/cypress/downloads/brew-planner-items-report.xlsx
+++ b/cypress/downloads/brew-planner-items-report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Reporte de Depósitos</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>salchicha</t>
-  </si>
-  <si>
-    <t>0.00</t>
   </si>
   <si>
     <t>Copyright © 2023 by BrewPlanner LLC</t>
@@ -254,16 +251,16 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7"/>
     <row r="8" s="6" customFormat="true">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>